<commit_message>
Incluindo restante dos arquivos referente ao commit anterior
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_bdd/dadosParaTeste/DadosParaTeste.xlsx
+++ b/src/main/java/br/com/rsinet/hub_bdd/dadosParaTeste/DadosParaTeste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Workspace\BDD\src\main\java\br\com\rsinet\hub_bdd\dataProvider\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Workspace\BDD\src\main\java\br\com\rsinet\hub_bdd\dadosParaTeste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFBFC17-8FF0-4604-AA5C-0FA59B23FF8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8182B749-1BA1-4903-B675-19DACE1C52A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
   </bookViews>
   <sheets>
     <sheet name="CenariosDeTeste" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Username</t>
   </si>
@@ -132,7 +132,22 @@
     <t>mouse hp</t>
   </si>
   <si>
-    <t>brotherhas</t>
+    <t>Clicar em produto</t>
+  </si>
+  <si>
+    <t>tablet</t>
+  </si>
+  <si>
+    <t>HP ELITEPAD 1000 G2 TABLET</t>
+  </si>
+  <si>
+    <t>notebook</t>
+  </si>
+  <si>
+    <t>HP ELITEBOOK FOLIO</t>
+  </si>
+  <si>
+    <t>ladygaga</t>
   </si>
 </sst>
 </file>
@@ -551,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -615,7 +630,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -692,10 +707,33 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
+      <c r="A7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="M8" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reestruturado todas as features e steps refatoradas.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_bdd/dadosParaTeste/DadosParaTeste.xlsx
+++ b/src/main/java/br/com/rsinet/hub_bdd/dadosParaTeste/DadosParaTeste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Workspace\BDD\src\main\java\br\com\rsinet\hub_bdd\dadosParaTeste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8182B749-1BA1-4903-B675-19DACE1C52A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40F0658-BFF7-4417-BDCF-46C1805275D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
   </bookViews>
@@ -147,7 +147,7 @@
     <t>HP ELITEBOOK FOLIO</t>
   </si>
   <si>
-    <t>ladygaga</t>
+    <t>qwjwejkfki</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Extent report com prints implementado
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_bdd/dadosParaTeste/DadosParaTeste.xlsx
+++ b/src/main/java/br/com/rsinet/hub_bdd/dadosParaTeste/DadosParaTeste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Workspace\BDD\src\main\java\br\com\rsinet\hub_bdd\dadosParaTeste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A74709-E1A0-4219-A2EE-8B7BC7E6F7F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20703DD-74FD-49D1-AAD5-F96949D3632E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23850" yWindow="3660" windowWidth="15375" windowHeight="7875" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
   </bookViews>
@@ -147,7 +147,7 @@
     <t>HP ELITEBOOK FOLIO</t>
   </si>
   <si>
-    <t>jkweiqwjk</t>
+    <t>asdfghhvm</t>
   </si>
 </sst>
 </file>

</xml_diff>